<commit_message>
Actualizacao do Load Data para trackerEntity
</commit_message>
<xml_diff>
--- a/data/data - Copy (2).xlsx
+++ b/data/data - Copy (2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felizardo Chaguala\Desktop\dhis2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2F20E9-4AE3-4CB7-A074-82A566301F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CEFDEC-6574-4EC8-8CFB-D2F4DAB998CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9F34BF02-54FC-45FB-A073-5E82DAD013A4}"/>
   </bookViews>
@@ -34,18 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>People who inject drugs (PWID)</t>
-  </si>
-  <si>
-    <t>Men who have sex with men (MSM)</t>
-  </si>
-  <si>
-    <t>Female sex workers (FSW)</t>
-  </si>
-  <si>
-    <t>People in prison and other closed settings</t>
+    <t>CT_TX_NEW - Breastfeeding</t>
   </si>
 </sst>
 </file>
@@ -449,50 +440,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACFA907-0D95-4933-814E-ACC98A48BE35}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="101" width="8.140625" style="1" customWidth="1"/>
-    <col min="102" max="102" width="12.5703125" style="1" customWidth="1"/>
-    <col min="103" max="106" width="9.5703125" style="1" customWidth="1"/>
-    <col min="107" max="107" width="8.140625" style="1" customWidth="1"/>
-    <col min="108" max="188" width="8.28515625" style="1"/>
-    <col min="189" max="189" width="9.7109375" style="1" customWidth="1"/>
-    <col min="190" max="16384" width="8.28515625" style="1"/>
+    <col min="1" max="1" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="98" width="8.140625" style="1" customWidth="1"/>
+    <col min="99" max="99" width="12.5703125" style="1" customWidth="1"/>
+    <col min="100" max="103" width="9.5703125" style="1" customWidth="1"/>
+    <col min="104" max="104" width="8.140625" style="1" customWidth="1"/>
+    <col min="105" max="185" width="8.28515625" style="1"/>
+    <col min="186" max="186" width="9.7109375" style="1" customWidth="1"/>
+    <col min="187" max="16384" width="8.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>